<commit_message>
updated occupancy files to fix occ_m2p bug. Now running full simulation
</commit_message>
<xml_diff>
--- a/Simulation_Tool/New_SimulationEnvironment/CEA_Archetypes_CH/results diagnosis.xlsx
+++ b/Simulation_Tool/New_SimulationEnvironment/CEA_Archetypes_CH/results diagnosis.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -91,6 +91,21 @@
   </si>
   <si>
     <t>CEA + occupancy_COM.csv</t>
+  </si>
+  <si>
+    <t>E      1182.148457</t>
+  </si>
+  <si>
+    <t>E_HCL  1891.341428</t>
+  </si>
+  <si>
+    <t>H       721.148026</t>
+  </si>
+  <si>
+    <t>L       326.172420</t>
+  </si>
+  <si>
+    <t>PV     -709.192971</t>
   </si>
 </sst>
 </file>
@@ -654,7 +669,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -666,6 +681,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -711,7 +727,17 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1052,10 +1078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:X31"/>
+  <dimension ref="B1:AF41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="F4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,8 +1091,8 @@
     <col min="26" max="26" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
@@ -1077,7 +1103,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -1098,30 +1124,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="8">
-        <v>3274.7595346799999</v>
+        <v>844.02</v>
       </c>
       <c r="D4" s="8">
-        <v>2895.23910209</v>
+        <v>1182.1400000000001</v>
       </c>
       <c r="E4" s="8">
-        <v>3675.21178306</v>
+        <v>1891.3</v>
       </c>
       <c r="F4" s="8">
-        <v>232.936536389</v>
+        <v>721.14800000000002</v>
       </c>
       <c r="G4" s="8">
-        <v>167.51571200000001</v>
+        <v>326.17200000000003</v>
       </c>
       <c r="H4" s="9">
-        <v>-779.97268097699998</v>
+        <v>-709</v>
       </c>
     </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
         <v>10</v>
       </c>
@@ -1144,7 +1170,7 @@
         <v>-766.94263414900001</v>
       </c>
     </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>21</v>
       </c>
@@ -1155,7 +1181,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>0</v>
       </c>
@@ -1219,8 +1245,29 @@
       <c r="X7" t="s">
         <v>6</v>
       </c>
+      <c r="Z7" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC7" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF7" s="11" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -1284,8 +1331,29 @@
       <c r="X8">
         <v>-774.85143084599997</v>
       </c>
+      <c r="Z8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA8" s="11">
+        <v>1000.98891688</v>
+      </c>
+      <c r="AB8" s="11">
+        <v>1892.71825268</v>
+      </c>
+      <c r="AC8" s="11">
+        <v>2608.5061435299999</v>
+      </c>
+      <c r="AD8" s="11">
+        <v>595.53688665000004</v>
+      </c>
+      <c r="AE8" s="11">
+        <v>1011.98034</v>
+      </c>
+      <c r="AF8" s="11">
+        <v>-715.78789085300002</v>
+      </c>
     </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -1349,8 +1417,29 @@
       <c r="X9">
         <v>-783.328473906</v>
       </c>
+      <c r="Z9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA9" s="11">
+        <v>2579.3956595200002</v>
+      </c>
+      <c r="AB9" s="11">
+        <v>2913.3116914100001</v>
+      </c>
+      <c r="AC9" s="11">
+        <v>3672.8187326900002</v>
+      </c>
+      <c r="AD9" s="11">
+        <v>276.75722316399998</v>
+      </c>
+      <c r="AE9" s="11">
+        <v>816.66584999999998</v>
+      </c>
+      <c r="AF9" s="11">
+        <v>-759.50704128300004</v>
+      </c>
     </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -1414,8 +1503,29 @@
       <c r="X10">
         <v>-771.54834180700004</v>
       </c>
+      <c r="Z10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA10" s="11">
+        <v>800.41735588400002</v>
+      </c>
+      <c r="AB10" s="11">
+        <v>3457.9145390200001</v>
+      </c>
+      <c r="AC10" s="11">
+        <v>4157.8228338199997</v>
+      </c>
+      <c r="AD10" s="11">
+        <v>1560.61712794</v>
+      </c>
+      <c r="AE10" s="11">
+        <v>1796.78835</v>
+      </c>
+      <c r="AF10" s="11">
+        <v>-699.90829480399998</v>
+      </c>
     </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>10</v>
       </c>
@@ -1479,8 +1589,29 @@
       <c r="X11">
         <v>-766.94263414900001</v>
       </c>
+      <c r="Z11" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA11" s="11">
+        <v>937.54697069899998</v>
+      </c>
+      <c r="AB11" s="11">
+        <v>1457.4020202300001</v>
+      </c>
+      <c r="AC11" s="11">
+        <v>2152.1351071099998</v>
+      </c>
+      <c r="AD11" s="11">
+        <v>976.80681641299998</v>
+      </c>
+      <c r="AE11" s="11">
+        <v>237.78131999999999</v>
+      </c>
+      <c r="AF11" s="11">
+        <v>-694.73308687700001</v>
+      </c>
     </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -1544,8 +1675,29 @@
       <c r="X12">
         <v>-772.47650672400005</v>
       </c>
+      <c r="Z12" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA12" s="11">
+        <v>743.18981422000002</v>
+      </c>
+      <c r="AB12" s="11">
+        <v>3444.2093039400002</v>
+      </c>
+      <c r="AC12" s="11">
+        <v>4141.9320063499999</v>
+      </c>
+      <c r="AD12" s="11">
+        <v>1632.08913613</v>
+      </c>
+      <c r="AE12" s="11">
+        <v>1766.6530560000001</v>
+      </c>
+      <c r="AF12" s="11">
+        <v>-697.72270241199999</v>
+      </c>
     </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -1609,8 +1761,29 @@
       <c r="X13">
         <v>-775.004078725</v>
       </c>
+      <c r="Z13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA13" s="11">
+        <v>1412.4201885499999</v>
+      </c>
+      <c r="AB13" s="11">
+        <v>1840.80425547</v>
+      </c>
+      <c r="AC13" s="11">
+        <v>2576.7181625399999</v>
+      </c>
+      <c r="AD13" s="11">
+        <v>544.58272399299995</v>
+      </c>
+      <c r="AE13" s="11">
+        <v>619.71524999999997</v>
+      </c>
+      <c r="AF13" s="11">
+        <v>-735.91390707799997</v>
+      </c>
     </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>13</v>
       </c>
@@ -1674,8 +1847,29 @@
       <c r="X14">
         <v>-772.78670124899998</v>
       </c>
+      <c r="Z14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA14" s="11">
+        <v>1029.35436998</v>
+      </c>
+      <c r="AB14" s="11">
+        <v>1932.4156518699999</v>
+      </c>
+      <c r="AC14" s="11">
+        <v>2647.0240278800002</v>
+      </c>
+      <c r="AD14" s="11">
+        <v>1077.4069279</v>
+      </c>
+      <c r="AE14" s="11">
+        <v>540.26273000000003</v>
+      </c>
+      <c r="AF14" s="11">
+        <v>-714.608376013</v>
+      </c>
     </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>14</v>
       </c>
@@ -1739,8 +1933,29 @@
       <c r="X15">
         <v>-762.43576466000002</v>
       </c>
+      <c r="Z15" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA15" s="11">
+        <v>2394.0773152800002</v>
+      </c>
+      <c r="AB15" s="11">
+        <v>2652.2502804199999</v>
+      </c>
+      <c r="AC15" s="11">
+        <v>3353.74844291</v>
+      </c>
+      <c r="AD15" s="11">
+        <v>677.04598763499996</v>
+      </c>
+      <c r="AE15" s="11">
+        <v>282.62513999999999</v>
+      </c>
+      <c r="AF15" s="11">
+        <v>-701.49816248699995</v>
+      </c>
     </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>15</v>
       </c>
@@ -1804,8 +2019,29 @@
       <c r="X16">
         <v>-767.98299274399994</v>
       </c>
+      <c r="Z16" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA16" s="11">
+        <v>1725.3032629100001</v>
+      </c>
+      <c r="AB16" s="11">
+        <v>3930.6776905500001</v>
+      </c>
+      <c r="AC16" s="11">
+        <v>4668.7127571999999</v>
+      </c>
+      <c r="AD16" s="11">
+        <v>969.75319428600005</v>
+      </c>
+      <c r="AE16" s="11">
+        <v>1973.6563000000001</v>
+      </c>
+      <c r="AF16" s="11">
+        <v>-738.03506664700001</v>
+      </c>
     </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>16</v>
       </c>
@@ -1869,8 +2105,29 @@
       <c r="X17">
         <v>-772.44990881399997</v>
       </c>
+      <c r="Z17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA17" s="11">
+        <v>649.03154109100001</v>
+      </c>
+      <c r="AB17" s="11">
+        <v>820.69634662099998</v>
+      </c>
+      <c r="AC17" s="11">
+        <v>1525.4270127699999</v>
+      </c>
+      <c r="AD17" s="11">
+        <v>792.36047168000005</v>
+      </c>
+      <c r="AE17" s="11">
+        <v>84.034999999999997</v>
+      </c>
+      <c r="AF17" s="11">
+        <v>-704.73066615000005</v>
+      </c>
     </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>17</v>
       </c>
@@ -1934,928 +2191,1303 @@
       <c r="X18">
         <v>-773.34226637500001</v>
       </c>
+      <c r="Z18" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA18" s="11">
+        <v>1321.0634699899999</v>
+      </c>
+      <c r="AB18" s="11">
+        <v>3551.1309077300002</v>
+      </c>
+      <c r="AC18" s="11">
+        <v>4292.7893989300001</v>
+      </c>
+      <c r="AD18" s="11">
+        <v>1137.9141589400001</v>
+      </c>
+      <c r="AE18" s="11">
+        <v>1833.81177</v>
+      </c>
+      <c r="AF18" s="11">
+        <v>-741.658491196</v>
+      </c>
     </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:32" x14ac:dyDescent="0.25">
       <c r="J20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>7</v>
       </c>
       <c r="C21">
         <f>C8-C$4</f>
-        <v>559.29969110999991</v>
+        <v>2990.0392257899998</v>
       </c>
       <c r="D21">
         <f t="shared" ref="D21:H21" si="0">D8-D$4</f>
-        <v>1269.6260254800004</v>
+        <v>2982.72512757</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>1263.1144560399998</v>
+        <v>3047.0262390999997</v>
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
-        <v>-140.64986307909999</v>
+        <v>-628.86132669009999</v>
       </c>
       <c r="G21">
         <f t="shared" si="0"/>
-        <v>844.46462799999995</v>
+        <v>685.80833999999993</v>
       </c>
       <c r="H21">
         <f t="shared" si="0"/>
-        <v>6.511569441000006</v>
+        <v>-64.461111535999976</v>
       </c>
       <c r="J21" t="s">
         <v>7</v>
       </c>
       <c r="K21">
-        <f t="shared" ref="K21:K31" si="1">K8-C$4</f>
-        <v>662.0843641700003</v>
+        <f>K8-C$4</f>
+        <v>3092.8238988500002</v>
       </c>
       <c r="L21">
-        <f t="shared" ref="L21:L31" si="2">L8-D$4</f>
-        <v>1404.8499741299997</v>
+        <f>L8-D$4</f>
+        <v>3117.9490762199994</v>
       </c>
       <c r="M21">
-        <f t="shared" ref="M21:M31" si="3">M8-E$4</f>
-        <v>1396.8939153199999</v>
+        <f>M8-E$4</f>
+        <v>3180.8056983799997</v>
       </c>
       <c r="N21">
-        <f t="shared" ref="N21:N31" si="4">N8-F$4</f>
-        <v>-109.65507686699999</v>
+        <f>N8-F$4</f>
+        <v>-597.86654047800005</v>
       </c>
       <c r="O21">
-        <f t="shared" ref="O21:O31" si="5">O8-G$4</f>
-        <v>844.46462799999995</v>
+        <f t="shared" ref="O21:O31" si="1">O8-G$4</f>
+        <v>685.80833999999993</v>
       </c>
       <c r="P21">
-        <f t="shared" ref="P21:P31" si="6">P8-H$4</f>
-        <v>7.9560588260000031</v>
+        <f t="shared" ref="P21:P31" si="2">P8-H$4</f>
+        <v>-63.016622150999979</v>
       </c>
       <c r="R21" t="s">
         <v>7</v>
       </c>
       <c r="S21">
-        <f t="shared" ref="S21:S31" si="7">S8-C$4</f>
-        <v>-134.05698961000007</v>
+        <f t="shared" ref="S21:S31" si="3">S8-C$4</f>
+        <v>2296.6825450699998</v>
       </c>
       <c r="T21">
-        <f t="shared" ref="T21:T31" si="8">T8-D$4</f>
-        <v>161.34457771999996</v>
+        <f t="shared" ref="T21:T31" si="4">T8-D$4</f>
+        <v>1874.4436798099998</v>
       </c>
       <c r="U21">
-        <f t="shared" ref="U21:U31" si="9">U8-E$4</f>
-        <v>156.22332758999983</v>
+        <f t="shared" ref="U21:U31" si="5">U8-E$4</f>
+        <v>1940.1351106499999</v>
       </c>
       <c r="V21">
-        <f t="shared" ref="V21:V31" si="10">V8-F$4</f>
-        <v>-89.312980807999992</v>
+        <f t="shared" ref="V21:V31" si="6">V8-F$4</f>
+        <v>-577.52444441900002</v>
       </c>
       <c r="W21">
-        <f t="shared" ref="W21:W31" si="11">W8-G$4</f>
-        <v>379.593298</v>
+        <f t="shared" ref="W21:W31" si="7">W8-G$4</f>
+        <v>220.93700999999999</v>
       </c>
       <c r="X21">
-        <f t="shared" ref="X21:X31" si="12">X8-H$4</f>
-        <v>5.1212501310000107</v>
+        <f t="shared" ref="X21:X31" si="8">X8-H$4</f>
+        <v>-65.851430845999971</v>
+      </c>
+      <c r="Z21" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA21" s="11">
+        <f>AA8-C$4</f>
+        <v>156.96891688000005</v>
+      </c>
+      <c r="AB21" s="11">
+        <f t="shared" ref="AB21:AF21" si="9">AB8-D$4</f>
+        <v>710.57825267999988</v>
+      </c>
+      <c r="AC21" s="11">
+        <f t="shared" si="9"/>
+        <v>717.20614352999996</v>
+      </c>
+      <c r="AD21" s="11">
+        <f t="shared" si="9"/>
+        <v>-125.61111334999998</v>
+      </c>
+      <c r="AE21" s="11">
+        <f t="shared" si="9"/>
+        <v>685.80833999999993</v>
+      </c>
+      <c r="AF21" s="11">
+        <f t="shared" si="9"/>
+        <v>-6.7878908530000217</v>
       </c>
     </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>8</v>
       </c>
       <c r="C22">
-        <f t="shared" ref="C22:H22" si="13">C9-C$4</f>
-        <v>7916.9750640200009</v>
+        <f t="shared" ref="C22:H22" si="10">C9-C$4</f>
+        <v>10347.7145987</v>
       </c>
       <c r="D22">
-        <f t="shared" si="13"/>
-        <v>8326.0766128100004</v>
+        <f t="shared" si="10"/>
+        <v>10039.1757149</v>
       </c>
       <c r="E22">
-        <f t="shared" si="13"/>
-        <v>8333.1886656400002</v>
+        <f t="shared" si="10"/>
+        <v>10117.100448700001</v>
       </c>
       <c r="F22">
-        <f t="shared" si="13"/>
-        <v>-232.936536389</v>
+        <f t="shared" si="10"/>
+        <v>-721.14800000000002</v>
       </c>
       <c r="G22">
-        <f t="shared" si="13"/>
-        <v>649.15013799999997</v>
+        <f t="shared" si="10"/>
+        <v>490.49384999999995</v>
       </c>
       <c r="H22">
-        <f t="shared" si="13"/>
-        <v>-7.1120528689999674</v>
+        <f t="shared" si="10"/>
+        <v>-78.084733845999949</v>
       </c>
       <c r="J22" t="s">
         <v>8</v>
       </c>
       <c r="K22">
+        <f>K9-C$4</f>
+        <v>10416.918876399999</v>
+      </c>
+      <c r="L22">
+        <f>L9-D$4</f>
+        <v>10108.6060827</v>
+      </c>
+      <c r="M22">
+        <f>M9-E$4</f>
+        <v>10186.5113695</v>
+      </c>
+      <c r="N22">
+        <f>N9-F$4</f>
+        <v>-720.94135689246605</v>
+      </c>
+      <c r="O22">
         <f t="shared" si="1"/>
-        <v>7986.1793417199997</v>
-      </c>
-      <c r="L22">
+        <v>490.49384999999995</v>
+      </c>
+      <c r="P22">
         <f t="shared" si="2"/>
-        <v>8395.50698061</v>
-      </c>
-      <c r="M22">
-        <f t="shared" si="3"/>
-        <v>8402.5995864399993</v>
-      </c>
-      <c r="N22">
-        <f t="shared" si="4"/>
-        <v>-232.72989328146599</v>
-      </c>
-      <c r="O22">
-        <f t="shared" si="5"/>
-        <v>649.15013799999997</v>
-      </c>
-      <c r="P22">
-        <f t="shared" si="6"/>
-        <v>-7.0926057579999906</v>
+        <v>-78.065286734999972</v>
       </c>
       <c r="R22" t="s">
         <v>8</v>
       </c>
       <c r="S22">
+        <f t="shared" si="3"/>
+        <v>3317.3729203199996</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="4"/>
+        <v>2426.6373127699999</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="5"/>
+        <v>2500.8057866700001</v>
+      </c>
+      <c r="V22">
+        <f t="shared" si="6"/>
+        <v>-631.69625364770002</v>
+      </c>
+      <c r="W22">
         <f t="shared" si="7"/>
-        <v>886.63338563999969</v>
-      </c>
-      <c r="T22">
+        <v>-184.91088000000002</v>
+      </c>
+      <c r="X22">
         <f t="shared" si="8"/>
-        <v>713.53821068000025</v>
-      </c>
-      <c r="U22">
-        <f t="shared" si="9"/>
-        <v>716.89400361000025</v>
-      </c>
-      <c r="V22">
-        <f t="shared" si="10"/>
-        <v>-143.48479003669999</v>
-      </c>
-      <c r="W22">
-        <f t="shared" si="11"/>
-        <v>-26.254592000000002</v>
-      </c>
-      <c r="X22">
-        <f t="shared" si="12"/>
-        <v>-3.3557929290000175</v>
+        <v>-74.328473905999999</v>
+      </c>
+      <c r="Z22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA22" s="11">
+        <f t="shared" ref="AA22:AA31" si="11">AA9-C$4</f>
+        <v>1735.3756595200002</v>
+      </c>
+      <c r="AB22" s="11">
+        <f t="shared" ref="AB22:AB31" si="12">AB9-D$4</f>
+        <v>1731.17169141</v>
+      </c>
+      <c r="AC22" s="11">
+        <f t="shared" ref="AC22:AC31" si="13">AC9-E$4</f>
+        <v>1781.5187326900002</v>
+      </c>
+      <c r="AD22" s="11">
+        <f t="shared" ref="AD22:AD31" si="14">AD9-F$4</f>
+        <v>-444.39077683600004</v>
+      </c>
+      <c r="AE22" s="11">
+        <f t="shared" ref="AE22:AE31" si="15">AE9-G$4</f>
+        <v>490.49384999999995</v>
+      </c>
+      <c r="AF22" s="11">
+        <f t="shared" ref="AF22:AF31" si="16">AF9-H$4</f>
+        <v>-50.507041283000035</v>
       </c>
     </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>9</v>
       </c>
       <c r="C23">
-        <f t="shared" ref="C23:H23" si="14">C10-C$4</f>
-        <v>13798.795261219999</v>
+        <f t="shared" ref="C23:H23" si="17">C10-C$4</f>
+        <v>16229.534795899999</v>
       </c>
       <c r="D23">
-        <f t="shared" si="14"/>
-        <v>15187.373323010001</v>
+        <f t="shared" si="17"/>
+        <v>16900.472425100001</v>
       </c>
       <c r="E23">
-        <f t="shared" si="14"/>
-        <v>15195.131362839998</v>
+        <f t="shared" si="17"/>
+        <v>16979.043145899999</v>
       </c>
       <c r="F23">
-        <f t="shared" si="14"/>
-        <v>-232.936536389</v>
+        <f t="shared" si="17"/>
+        <v>-721.14800000000002</v>
       </c>
       <c r="G23">
-        <f t="shared" si="14"/>
-        <v>1629.2726379999999</v>
+        <f t="shared" si="17"/>
+        <v>1470.61635</v>
       </c>
       <c r="H23">
-        <f t="shared" si="14"/>
-        <v>-7.7580397799999901</v>
+        <f t="shared" si="17"/>
+        <v>-78.730720756999972</v>
       </c>
       <c r="J23" t="s">
         <v>9</v>
       </c>
       <c r="K23">
+        <f>K10-C$4</f>
+        <v>16243.6449407</v>
+      </c>
+      <c r="L23">
+        <f>L10-D$4</f>
+        <v>16914.590919900002</v>
+      </c>
+      <c r="M23">
+        <f>M10-E$4</f>
+        <v>16993.1532907</v>
+      </c>
+      <c r="N23">
+        <f>N10-F$4</f>
+        <v>-721.14800000000002</v>
+      </c>
+      <c r="O23">
         <f t="shared" si="1"/>
-        <v>13812.90540602</v>
-      </c>
-      <c r="L23">
+        <v>1470.61635</v>
+      </c>
+      <c r="P23">
         <f t="shared" si="2"/>
-        <v>15201.491817810002</v>
-      </c>
-      <c r="M23">
-        <f t="shared" si="3"/>
-        <v>15209.241507639999</v>
-      </c>
-      <c r="N23">
-        <f t="shared" si="4"/>
-        <v>-232.936536389</v>
-      </c>
-      <c r="O23">
-        <f t="shared" si="5"/>
-        <v>1629.2726379999999</v>
-      </c>
-      <c r="P23">
-        <f t="shared" si="6"/>
-        <v>-7.7496898420000662</v>
+        <v>-78.722370819000048</v>
       </c>
       <c r="R23" t="s">
         <v>9</v>
       </c>
       <c r="S23">
+        <f t="shared" si="3"/>
+        <v>2295.9398091500002</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="4"/>
+        <v>1655.3106957399998</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="5"/>
+        <v>1717.6990375500002</v>
+      </c>
+      <c r="V23">
+        <f t="shared" si="6"/>
+        <v>-386.44472160500004</v>
+      </c>
+      <c r="W23">
         <f t="shared" si="7"/>
-        <v>-134.79972552999971</v>
-      </c>
-      <c r="T23">
+        <v>-191.83605000000003</v>
+      </c>
+      <c r="X23">
         <f t="shared" si="8"/>
-        <v>-57.788406350000059</v>
-      </c>
-      <c r="U23">
-        <f t="shared" si="9"/>
-        <v>-66.212745509999877</v>
-      </c>
-      <c r="V23">
-        <f t="shared" si="10"/>
-        <v>101.76674200599999</v>
-      </c>
-      <c r="W23">
+        <v>-62.548341807000043</v>
+      </c>
+      <c r="Z23" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA23" s="11">
         <f t="shared" si="11"/>
-        <v>-33.179762000000011</v>
-      </c>
-      <c r="X23">
+        <v>-43.602644115999965</v>
+      </c>
+      <c r="AB23" s="11">
         <f t="shared" si="12"/>
-        <v>8.4243391699999393</v>
+        <v>2275.7745390199998</v>
+      </c>
+      <c r="AC23" s="11">
+        <f t="shared" si="13"/>
+        <v>2266.5228338199995</v>
+      </c>
+      <c r="AD23" s="11">
+        <f t="shared" si="14"/>
+        <v>839.46912794000002</v>
+      </c>
+      <c r="AE23" s="11">
+        <f t="shared" si="15"/>
+        <v>1470.61635</v>
+      </c>
+      <c r="AF23" s="11">
+        <f t="shared" si="16"/>
+        <v>9.0917051960000208</v>
       </c>
     </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C24" s="10">
-        <f t="shared" ref="C24:H24" si="15">C11-C$4</f>
-        <v>390.86775500000022</v>
+        <f t="shared" ref="C24:H24" si="18">C11-C$4</f>
+        <v>2821.6072896800001</v>
       </c>
       <c r="D24" s="10">
-        <f t="shared" si="15"/>
-        <v>489.2956399499999</v>
+        <f t="shared" si="18"/>
+        <v>2202.39474204</v>
       </c>
       <c r="E24" s="10">
-        <f t="shared" si="15"/>
-        <v>476.26559312999962</v>
+        <f t="shared" si="18"/>
+        <v>2260.1773761899994</v>
       </c>
       <c r="F24" s="10">
-        <f t="shared" si="15"/>
-        <v>15.132230124000017</v>
+        <f t="shared" si="18"/>
+        <v>-473.07923348700001</v>
       </c>
       <c r="G24" s="10">
-        <f t="shared" si="15"/>
-        <v>70.265607999999986</v>
+        <f t="shared" si="18"/>
+        <v>-88.390680000000032</v>
       </c>
       <c r="H24" s="10">
-        <f t="shared" si="15"/>
-        <v>13.030046827999968</v>
+        <f t="shared" si="18"/>
+        <v>-57.942634149000014</v>
       </c>
       <c r="J24" t="s">
         <v>10</v>
       </c>
       <c r="K24">
+        <f t="shared" ref="K24:K31" si="19">K11-C$4</f>
+        <v>2954.5894792300001</v>
+      </c>
+      <c r="L24">
+        <f t="shared" ref="L24:L31" si="20">L11-D$4</f>
+        <v>2367.0822263199998</v>
+      </c>
+      <c r="M24">
+        <f t="shared" ref="M24:M31" si="21">M11-E$4</f>
+        <v>2424.7170249000001</v>
+      </c>
+      <c r="N24">
+        <f t="shared" ref="N24:N31" si="22">N11-F$4</f>
+        <v>-441.52177433000003</v>
+      </c>
+      <c r="O24">
         <f t="shared" si="1"/>
-        <v>523.84994455000015</v>
-      </c>
-      <c r="L24">
+        <v>-88.390680000000032</v>
+      </c>
+      <c r="P24">
         <f t="shared" si="2"/>
-        <v>653.98312423000016</v>
-      </c>
-      <c r="M24">
-        <f t="shared" si="3"/>
-        <v>640.80524184000024</v>
-      </c>
-      <c r="N24">
-        <f t="shared" si="4"/>
-        <v>46.689689281</v>
-      </c>
-      <c r="O24">
-        <f t="shared" si="5"/>
-        <v>70.265607999999986</v>
-      </c>
-      <c r="P24">
-        <f t="shared" si="6"/>
-        <v>13.177882394999983</v>
+        <v>-57.794798581999999</v>
       </c>
       <c r="R24" t="s">
         <v>10</v>
       </c>
       <c r="S24">
+        <f t="shared" si="3"/>
+        <v>2821.6072896800001</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="4"/>
+        <v>2202.39474204</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="5"/>
+        <v>2260.1773761899994</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="6"/>
+        <v>-473.07923348700001</v>
+      </c>
+      <c r="W24">
         <f t="shared" si="7"/>
-        <v>390.86775500000022</v>
-      </c>
-      <c r="T24">
+        <v>-88.390680000000032</v>
+      </c>
+      <c r="X24">
         <f t="shared" si="8"/>
-        <v>489.2956399499999</v>
-      </c>
-      <c r="U24">
-        <f t="shared" si="9"/>
-        <v>476.26559312999962</v>
-      </c>
-      <c r="V24">
-        <f t="shared" si="10"/>
-        <v>15.132230124000017</v>
-      </c>
-      <c r="W24">
-        <f t="shared" si="11"/>
-        <v>70.265607999999986</v>
-      </c>
-      <c r="X24">
+        <v>-57.942634149000014</v>
+      </c>
+      <c r="Z24" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA24" s="11">
+        <f>AA11-C$4</f>
+        <v>93.526970699000003</v>
+      </c>
+      <c r="AB24" s="11">
         <f t="shared" si="12"/>
-        <v>13.030046827999968</v>
+        <v>275.26202022999996</v>
+      </c>
+      <c r="AC24" s="11">
+        <f t="shared" si="13"/>
+        <v>260.83510710999985</v>
+      </c>
+      <c r="AD24" s="11">
+        <f t="shared" si="14"/>
+        <v>255.65881641299995</v>
+      </c>
+      <c r="AE24" s="11">
+        <f t="shared" si="15"/>
+        <v>-88.390680000000032</v>
+      </c>
+      <c r="AF24" s="11">
+        <f t="shared" si="16"/>
+        <v>14.266913122999995</v>
       </c>
     </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>11</v>
       </c>
       <c r="C25">
-        <f t="shared" ref="C25:H25" si="16">C12-C$4</f>
-        <v>13782.330630419998</v>
+        <f t="shared" ref="C25:H25" si="23">C12-C$4</f>
+        <v>16213.070165099998</v>
       </c>
       <c r="D25">
-        <f t="shared" si="16"/>
-        <v>15138.71828641</v>
+        <f t="shared" si="23"/>
+        <v>16851.8173885</v>
       </c>
       <c r="E25">
-        <f t="shared" si="16"/>
-        <v>15148.531438040001</v>
+        <f t="shared" si="23"/>
+        <v>16932.443221100002</v>
       </c>
       <c r="F25">
-        <f t="shared" si="16"/>
-        <v>-232.936536389</v>
+        <f t="shared" si="23"/>
+        <v>-721.14800000000002</v>
       </c>
       <c r="G25">
-        <f t="shared" si="16"/>
-        <v>1599.1373440000002</v>
+        <f t="shared" si="23"/>
+        <v>1440.4810560000001</v>
       </c>
       <c r="H25">
-        <f t="shared" si="16"/>
-        <v>-9.8131515630000195</v>
+        <f t="shared" si="23"/>
+        <v>-80.785832540000001</v>
       </c>
       <c r="J25" t="s">
         <v>11</v>
       </c>
       <c r="K25">
+        <f t="shared" si="19"/>
+        <v>16227.0938513</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="20"/>
+        <v>16865.8591227</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="21"/>
+        <v>16946.4669073</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="22"/>
+        <v>-721.14800000000002</v>
+      </c>
+      <c r="O25">
         <f t="shared" si="1"/>
-        <v>13796.35431662</v>
-      </c>
-      <c r="L25">
+        <v>1440.4810560000001</v>
+      </c>
+      <c r="P25">
         <f t="shared" si="2"/>
-        <v>15152.76002061</v>
-      </c>
-      <c r="M25">
-        <f t="shared" si="3"/>
-        <v>15162.55512424</v>
-      </c>
-      <c r="N25">
-        <f t="shared" si="4"/>
-        <v>-232.936536389</v>
-      </c>
-      <c r="O25">
-        <f t="shared" si="5"/>
-        <v>1599.1373440000002</v>
-      </c>
-      <c r="P25">
-        <f t="shared" si="6"/>
-        <v>-9.7951036489999979</v>
+        <v>-80.76778462599998</v>
       </c>
       <c r="R25" t="s">
         <v>11</v>
       </c>
       <c r="S25">
+        <f t="shared" si="3"/>
+        <v>2292.0553941500002</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="4"/>
+        <v>1644.2283718199999</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="5"/>
+        <v>1707.5448785400001</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="6"/>
+        <v>-384.67111561000002</v>
+      </c>
+      <c r="W25">
         <f t="shared" si="7"/>
-        <v>-138.68414052999969</v>
-      </c>
-      <c r="T25">
+        <v>-199.87940000000003</v>
+      </c>
+      <c r="X25">
         <f t="shared" si="8"/>
-        <v>-68.870730269999967</v>
-      </c>
-      <c r="U25">
-        <f t="shared" si="9"/>
-        <v>-76.366904519999935</v>
-      </c>
-      <c r="V25">
-        <f t="shared" si="10"/>
-        <v>103.54034800100001</v>
-      </c>
-      <c r="W25">
+        <v>-63.476506724000046</v>
+      </c>
+      <c r="Z25" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA25" s="11">
         <f t="shared" si="11"/>
-        <v>-41.223112000000015</v>
-      </c>
-      <c r="X25">
+        <v>-100.83018577999997</v>
+      </c>
+      <c r="AB25" s="11">
         <f t="shared" si="12"/>
-        <v>7.4961742529999356</v>
+        <v>2262.0693039400003</v>
+      </c>
+      <c r="AC25" s="11">
+        <f t="shared" si="13"/>
+        <v>2250.6320063499998</v>
+      </c>
+      <c r="AD25" s="11">
+        <f t="shared" si="14"/>
+        <v>910.94113613000002</v>
+      </c>
+      <c r="AE25" s="11">
+        <f t="shared" si="15"/>
+        <v>1440.4810560000001</v>
+      </c>
+      <c r="AF25" s="11">
+        <f t="shared" si="16"/>
+        <v>11.27729758800001</v>
       </c>
     </row>
-    <row r="26" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>12</v>
       </c>
       <c r="C26">
-        <f t="shared" ref="C26:H26" si="17">C13-C$4</f>
-        <v>-341.36571366999988</v>
+        <f t="shared" ref="C26:H26" si="24">C13-C$4</f>
+        <v>2089.37382101</v>
       </c>
       <c r="D26">
-        <f t="shared" si="17"/>
-        <v>97.020147619999989</v>
+        <f t="shared" si="24"/>
+        <v>1810.1192497099998</v>
       </c>
       <c r="E26">
-        <f t="shared" si="17"/>
-        <v>81.404653749999852</v>
+        <f t="shared" si="24"/>
+        <v>1865.3164368099999</v>
       </c>
       <c r="F26">
-        <f t="shared" si="17"/>
-        <v>-29.429170591000002</v>
+        <f t="shared" si="24"/>
+        <v>-517.640634202</v>
       </c>
       <c r="G26">
-        <f t="shared" si="17"/>
-        <v>452.19953799999996</v>
+        <f t="shared" si="24"/>
+        <v>293.54324999999994</v>
       </c>
       <c r="H26">
-        <f t="shared" si="17"/>
-        <v>15.615493876999949</v>
+        <f t="shared" si="24"/>
+        <v>-55.357187100000033</v>
       </c>
       <c r="J26" t="s">
         <v>12</v>
       </c>
       <c r="K26">
+        <f t="shared" si="19"/>
+        <v>2147.8958533300001</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="20"/>
+        <v>1885.27873849</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="21"/>
+        <v>1940.1495802400002</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="22"/>
+        <v>-501.32952308900002</v>
+      </c>
+      <c r="O26">
         <f t="shared" si="1"/>
-        <v>-282.84368134999977</v>
-      </c>
-      <c r="L26">
+        <v>293.54324999999994</v>
+      </c>
+      <c r="P26">
         <f t="shared" si="2"/>
-        <v>172.17963640000016</v>
-      </c>
-      <c r="M26">
-        <f t="shared" si="3"/>
-        <v>156.23779718000014</v>
-      </c>
-      <c r="N26">
-        <f t="shared" si="4"/>
-        <v>-13.118059477999992</v>
-      </c>
-      <c r="O26">
-        <f t="shared" si="5"/>
-        <v>452.19953799999996</v>
-      </c>
-      <c r="P26">
-        <f t="shared" si="6"/>
-        <v>15.941839225999956</v>
+        <v>-55.030841751000025</v>
       </c>
       <c r="R26" t="s">
         <v>12</v>
       </c>
       <c r="S26">
+        <f t="shared" si="3"/>
+        <v>2060.1185256100002</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="4"/>
+        <v>1234.8139576999999</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="5"/>
+        <v>1300.6580364200001</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="6"/>
+        <v>-538.87816418300008</v>
+      </c>
+      <c r="W26">
         <f t="shared" si="7"/>
-        <v>-370.62100906999967</v>
-      </c>
-      <c r="T26">
+        <v>-220.62232500000005</v>
+      </c>
+      <c r="X26">
         <f t="shared" si="8"/>
-        <v>-478.28514438999991</v>
-      </c>
-      <c r="U26">
-        <f t="shared" si="9"/>
-        <v>-483.25374663999992</v>
-      </c>
-      <c r="V26">
-        <f t="shared" si="10"/>
-        <v>-50.666700571999996</v>
-      </c>
-      <c r="W26">
+        <v>-66.004078724999999</v>
+      </c>
+      <c r="Z26" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA26" s="11">
         <f t="shared" si="11"/>
-        <v>-61.966037000000014</v>
-      </c>
-      <c r="X26">
+        <v>568.40018854999994</v>
+      </c>
+      <c r="AB26" s="11">
         <f t="shared" si="12"/>
-        <v>4.9686022519999824</v>
+        <v>658.66425546999994</v>
+      </c>
+      <c r="AC26" s="11">
+        <f t="shared" si="13"/>
+        <v>685.41816253999991</v>
+      </c>
+      <c r="AD26" s="11">
+        <f t="shared" si="14"/>
+        <v>-176.56527600700008</v>
+      </c>
+      <c r="AE26" s="11">
+        <f t="shared" si="15"/>
+        <v>293.54324999999994</v>
+      </c>
+      <c r="AF26" s="11">
+        <f t="shared" si="16"/>
+        <v>-26.913907077999966</v>
       </c>
     </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>13</v>
       </c>
       <c r="C27">
-        <f t="shared" ref="C27:H27" si="18">C14-C$4</f>
-        <v>5284.0109920700006</v>
+        <f t="shared" ref="C27:H27" si="25">C14-C$4</f>
+        <v>7714.7505267500001</v>
       </c>
       <c r="D27">
-        <f t="shared" si="18"/>
-        <v>5421.69851973</v>
+        <f t="shared" si="25"/>
+        <v>7134.7976218199992</v>
       </c>
       <c r="E27">
-        <f t="shared" si="18"/>
-        <v>5427.2293408200003</v>
+        <f t="shared" si="25"/>
+        <v>7211.1411238800001</v>
       </c>
       <c r="F27">
-        <f t="shared" si="18"/>
-        <v>-229.52866926464</v>
+        <f t="shared" si="25"/>
+        <v>-717.74013287564003</v>
       </c>
       <c r="G27">
-        <f t="shared" si="18"/>
-        <v>372.74701800000003</v>
+        <f t="shared" si="25"/>
+        <v>214.09073000000001</v>
       </c>
       <c r="H27">
-        <f t="shared" si="18"/>
-        <v>-5.530821082999978</v>
+        <f t="shared" si="25"/>
+        <v>-76.50350205999996</v>
       </c>
       <c r="J27" t="s">
         <v>13</v>
       </c>
       <c r="K27">
+        <f t="shared" si="19"/>
+        <v>7736.9428429999989</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="20"/>
+        <v>7161.0884728400006</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="21"/>
+        <v>7237.1920973099996</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="22"/>
+        <v>-713.88147569085004</v>
+      </c>
+      <c r="O27">
         <f t="shared" si="1"/>
-        <v>5306.2033083199995</v>
-      </c>
-      <c r="L27">
+        <v>214.09073000000001</v>
+      </c>
+      <c r="P27">
         <f t="shared" si="2"/>
-        <v>5447.9893707500014</v>
-      </c>
-      <c r="M27">
-        <f t="shared" si="3"/>
-        <v>5453.2803142499997</v>
-      </c>
-      <c r="N27">
-        <f t="shared" si="4"/>
-        <v>-225.67001207984998</v>
-      </c>
-      <c r="O27">
-        <f t="shared" si="5"/>
-        <v>372.74701800000003</v>
-      </c>
-      <c r="P27">
-        <f t="shared" si="6"/>
-        <v>-5.2909434919999967</v>
+        <v>-76.263624468999978</v>
       </c>
       <c r="R27" t="s">
         <v>13</v>
       </c>
       <c r="S27">
+        <f t="shared" si="3"/>
+        <v>2339.7849268</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="4"/>
+        <v>1880.39999564</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="5"/>
+        <v>1944.0266968900003</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="6"/>
+        <v>-113.85950990399999</v>
+      </c>
+      <c r="W27">
         <f t="shared" si="7"/>
-        <v>-90.954607879999912</v>
-      </c>
-      <c r="T27">
+        <v>-281.93872000000005</v>
+      </c>
+      <c r="X27">
         <f t="shared" si="8"/>
-        <v>167.30089355000018</v>
-      </c>
-      <c r="U27">
-        <f t="shared" si="9"/>
-        <v>160.11491383000021</v>
-      </c>
-      <c r="V27">
-        <f t="shared" si="10"/>
-        <v>374.35195370700001</v>
-      </c>
-      <c r="W27">
+        <v>-63.786701248999975</v>
+      </c>
+      <c r="Z27" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA27" s="11">
         <f t="shared" si="11"/>
-        <v>-123.282432</v>
-      </c>
-      <c r="X27">
+        <v>185.33436998000002</v>
+      </c>
+      <c r="AB27" s="11">
         <f t="shared" si="12"/>
-        <v>7.1859797280000066</v>
+        <v>750.27565186999982</v>
+      </c>
+      <c r="AC27" s="11">
+        <f t="shared" si="13"/>
+        <v>755.72402788000022</v>
+      </c>
+      <c r="AD27" s="11">
+        <f t="shared" si="14"/>
+        <v>356.2589279</v>
+      </c>
+      <c r="AE27" s="11">
+        <f t="shared" si="15"/>
+        <v>214.09073000000001</v>
+      </c>
+      <c r="AF27" s="11">
+        <f t="shared" si="16"/>
+        <v>-5.6083760129999973</v>
       </c>
     </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>14</v>
       </c>
       <c r="C28">
-        <f t="shared" ref="C28:H28" si="19">C15-C$4</f>
-        <v>1961.4917618999998</v>
+        <f t="shared" ref="C28:H28" si="26">C15-C$4</f>
+        <v>4392.2312965799993</v>
       </c>
       <c r="D28">
-        <f t="shared" si="19"/>
-        <v>2100.5750720999999</v>
+        <f t="shared" si="26"/>
+        <v>3813.6741741899996</v>
       </c>
       <c r="E28">
-        <f t="shared" si="19"/>
-        <v>2076.5291033499998</v>
+        <f t="shared" si="26"/>
+        <v>3860.4408864099996</v>
       </c>
       <c r="F28">
-        <f t="shared" si="19"/>
-        <v>-7.2086560999991889E-2</v>
+        <f t="shared" si="26"/>
+        <v>-488.28355017199999</v>
       </c>
       <c r="G28">
-        <f t="shared" si="19"/>
-        <v>115.10942799999998</v>
+        <f t="shared" si="26"/>
+        <v>-43.546860000000038</v>
       </c>
       <c r="H28">
-        <f t="shared" si="19"/>
-        <v>24.04596875499999</v>
+        <f t="shared" si="26"/>
+        <v>-46.926712221999992</v>
       </c>
       <c r="J28" t="s">
         <v>14</v>
       </c>
       <c r="K28">
+        <f t="shared" si="19"/>
+        <v>4519.6511385499998</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="20"/>
+        <v>3996.7323513299998</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="21"/>
+        <v>4043.2298177399998</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="22"/>
+        <v>-432.91446081300001</v>
+      </c>
+      <c r="O28">
         <f t="shared" si="1"/>
-        <v>2088.9116038700004</v>
-      </c>
-      <c r="L28">
+        <v>-43.546860000000038</v>
+      </c>
+      <c r="P28">
         <f t="shared" si="2"/>
-        <v>2283.6332492400002</v>
-      </c>
-      <c r="M28">
-        <f t="shared" si="3"/>
-        <v>2259.31803468</v>
-      </c>
-      <c r="N28">
-        <f t="shared" si="4"/>
-        <v>55.297002798000022</v>
-      </c>
-      <c r="O28">
-        <f t="shared" si="5"/>
-        <v>115.10942799999998</v>
-      </c>
-      <c r="P28">
-        <f t="shared" si="6"/>
-        <v>24.315214562999927</v>
+        <v>-46.657466414000055</v>
       </c>
       <c r="R28" t="s">
         <v>14</v>
       </c>
       <c r="S28">
+        <f t="shared" si="3"/>
+        <v>3459.2508162099998</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="4"/>
+        <v>2802.8919718899997</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="5"/>
+        <v>2856.16773655</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="6"/>
+        <v>-429.74728966000004</v>
+      </c>
+      <c r="W28">
         <f t="shared" si="7"/>
-        <v>1028.5112815299999</v>
-      </c>
-      <c r="T28">
+        <v>-173.37579000000002</v>
+      </c>
+      <c r="X28">
         <f t="shared" si="8"/>
-        <v>1089.7928698000001</v>
-      </c>
-      <c r="U28">
-        <f t="shared" si="9"/>
-        <v>1072.2559534900001</v>
-      </c>
-      <c r="V28">
-        <f t="shared" si="10"/>
-        <v>58.464173950999992</v>
-      </c>
-      <c r="W28">
+        <v>-53.435764660000018</v>
+      </c>
+      <c r="Z28" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA28" s="11">
         <f t="shared" si="11"/>
-        <v>-14.719502000000006</v>
-      </c>
-      <c r="X28">
+        <v>1550.0573152800002</v>
+      </c>
+      <c r="AB28" s="11">
         <f t="shared" si="12"/>
-        <v>17.536916316999964</v>
+        <v>1470.1102804199998</v>
+      </c>
+      <c r="AC28" s="11">
+        <f t="shared" si="13"/>
+        <v>1462.44844291</v>
+      </c>
+      <c r="AD28" s="11">
+        <f t="shared" si="14"/>
+        <v>-44.102012365000064</v>
+      </c>
+      <c r="AE28" s="11">
+        <f t="shared" si="15"/>
+        <v>-43.546860000000038</v>
+      </c>
+      <c r="AF28" s="11">
+        <f t="shared" si="16"/>
+        <v>7.501837513000055</v>
       </c>
     </row>
-    <row r="29" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>15</v>
       </c>
       <c r="C29">
-        <f t="shared" ref="C29:H29" si="20">C16-C$4</f>
-        <v>14429.409447819999</v>
+        <f t="shared" ref="C29:H29" si="27">C16-C$4</f>
+        <v>16860.148982499999</v>
       </c>
       <c r="D29">
-        <f t="shared" si="20"/>
-        <v>16005.452676410001</v>
+        <f t="shared" si="27"/>
+        <v>17718.551778500001</v>
       </c>
       <c r="E29">
-        <f t="shared" si="20"/>
-        <v>16003.634224040001</v>
+        <f t="shared" si="27"/>
+        <v>17787.546007100002</v>
       </c>
       <c r="F29">
-        <f t="shared" si="20"/>
-        <v>-231.91581177693999</v>
+        <f t="shared" si="27"/>
+        <v>-720.12727538794002</v>
       </c>
       <c r="G29">
-        <f t="shared" si="20"/>
-        <v>1806.1405880000002</v>
+        <f t="shared" si="27"/>
+        <v>1647.4843000000001</v>
       </c>
       <c r="H29">
-        <f t="shared" si="20"/>
-        <v>1.8184524399999873</v>
+        <f t="shared" si="27"/>
+        <v>-69.154228536999995</v>
       </c>
       <c r="J29" t="s">
         <v>15</v>
       </c>
       <c r="K29">
+        <f t="shared" si="19"/>
+        <v>16876.111185099999</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="20"/>
+        <v>17734.148545100001</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="21"/>
+        <v>17803.134739600002</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="22"/>
+        <v>-720.50074551523107</v>
+      </c>
+      <c r="O29">
         <f t="shared" si="1"/>
-        <v>14445.371650419998</v>
-      </c>
-      <c r="L29">
+        <v>1647.4843000000001</v>
+      </c>
+      <c r="P29">
         <f t="shared" si="2"/>
-        <v>16021.049443010001</v>
-      </c>
-      <c r="M29">
-        <f t="shared" si="3"/>
-        <v>16019.222956540001</v>
-      </c>
-      <c r="N29">
-        <f t="shared" si="4"/>
-        <v>-232.28928190423099</v>
-      </c>
-      <c r="O29">
-        <f t="shared" si="5"/>
-        <v>1806.1405880000002</v>
-      </c>
-      <c r="P29">
-        <f t="shared" si="6"/>
-        <v>1.8264864980000084</v>
+        <v>-69.146194478999973</v>
       </c>
       <c r="R29" t="s">
         <v>15</v>
       </c>
       <c r="S29">
+        <f t="shared" si="3"/>
+        <v>2363.00013786</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="4"/>
+        <v>2049.1050576799998</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="5"/>
+        <v>2107.9280504199996</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="6"/>
+        <v>-109.66678744199999</v>
+      </c>
+      <c r="W29">
         <f t="shared" si="7"/>
-        <v>-67.739396819999911</v>
-      </c>
-      <c r="T29">
+        <v>-145.44530000000003</v>
+      </c>
+      <c r="X29">
         <f t="shared" si="8"/>
-        <v>336.00595559000021</v>
-      </c>
-      <c r="U29">
-        <f t="shared" si="9"/>
-        <v>324.0162673599998</v>
-      </c>
-      <c r="V29">
-        <f t="shared" si="10"/>
-        <v>378.54467616900001</v>
-      </c>
-      <c r="W29">
+        <v>-58.982992743999944</v>
+      </c>
+      <c r="Z29" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA29" s="11">
         <f t="shared" si="11"/>
-        <v>13.210987999999986</v>
-      </c>
-      <c r="X29">
+        <v>881.28326291000008</v>
+      </c>
+      <c r="AB29" s="11">
         <f t="shared" si="12"/>
-        <v>11.989688233000038</v>
+        <v>2748.5376905499998</v>
+      </c>
+      <c r="AC29" s="11">
+        <f t="shared" si="13"/>
+        <v>2777.4127571999998</v>
+      </c>
+      <c r="AD29" s="11">
+        <f t="shared" si="14"/>
+        <v>248.60519428600003</v>
+      </c>
+      <c r="AE29" s="11">
+        <f t="shared" si="15"/>
+        <v>1647.4843000000001</v>
+      </c>
+      <c r="AF29" s="11">
+        <f t="shared" si="16"/>
+        <v>-29.035066647000008</v>
       </c>
     </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>16</v>
       </c>
       <c r="C30">
-        <f t="shared" ref="C30:H30" si="21">C17-C$4</f>
-        <v>-1017.0726877100001</v>
+        <f t="shared" ref="C30:H30" si="28">C17-C$4</f>
+        <v>1413.6668469699998</v>
       </c>
       <c r="D30">
-        <f t="shared" si="21"/>
-        <v>-1146.3351428999999</v>
+        <f t="shared" si="28"/>
+        <v>566.76395918999992</v>
       </c>
       <c r="E30">
-        <f t="shared" si="21"/>
-        <v>-1159.2753163100001</v>
+        <f t="shared" si="28"/>
+        <v>624.63646674999995</v>
       </c>
       <c r="F30">
-        <f t="shared" si="21"/>
-        <v>-58.721916609000004</v>
+        <f t="shared" si="28"/>
+        <v>-546.93338022</v>
       </c>
       <c r="G30">
-        <f t="shared" si="21"/>
-        <v>-83.480712000000011</v>
+        <f t="shared" si="28"/>
+        <v>-242.13700000000003</v>
       </c>
       <c r="H30">
-        <f t="shared" si="21"/>
-        <v>12.940173416999983</v>
+        <f t="shared" si="28"/>
+        <v>-58.032507559999999</v>
       </c>
       <c r="J30" t="s">
         <v>16</v>
       </c>
       <c r="K30">
+        <f t="shared" si="19"/>
+        <v>1519.7414156300001</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="20"/>
+        <v>703.70673812999985</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="21"/>
+        <v>762.43645889000004</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="22"/>
+        <v>-515.20795673999999</v>
+      </c>
+      <c r="O30">
         <f t="shared" si="1"/>
-        <v>-910.99811904999979</v>
-      </c>
-      <c r="L30">
+        <v>-242.13700000000003</v>
+      </c>
+      <c r="P30">
         <f t="shared" si="2"/>
-        <v>-1009.39236396</v>
-      </c>
-      <c r="M30">
-        <f t="shared" si="3"/>
-        <v>-1021.47532417</v>
-      </c>
-      <c r="N30">
-        <f t="shared" si="4"/>
-        <v>-26.996493128999987</v>
-      </c>
-      <c r="O30">
-        <f t="shared" si="5"/>
-        <v>-83.480712000000011</v>
-      </c>
-      <c r="P30">
-        <f t="shared" si="6"/>
-        <v>12.082960212999978</v>
+        <v>-58.889720764000003</v>
       </c>
       <c r="R30" t="s">
         <v>16</v>
       </c>
       <c r="S30">
+        <f t="shared" si="3"/>
+        <v>2292.9121259500002</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="4"/>
+        <v>1575.5227525399998</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="5"/>
+        <v>1638.8126613500001</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="6"/>
+        <v>-537.33466459900001</v>
+      </c>
+      <c r="W30">
         <f t="shared" si="7"/>
-        <v>-137.82740872999966</v>
-      </c>
-      <c r="T30">
+        <v>-116.80480000000003</v>
+      </c>
+      <c r="X30">
         <f t="shared" si="8"/>
-        <v>-137.57634955000003</v>
-      </c>
-      <c r="U30">
-        <f t="shared" si="9"/>
-        <v>-145.09912170999996</v>
-      </c>
-      <c r="V30">
-        <f t="shared" si="10"/>
-        <v>-49.123200988000008</v>
-      </c>
-      <c r="W30">
+        <v>-63.449908813999969</v>
+      </c>
+      <c r="Z30" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA30" s="11">
         <f t="shared" si="11"/>
-        <v>41.851487999999989</v>
-      </c>
-      <c r="X30">
+        <v>-194.98845890899997</v>
+      </c>
+      <c r="AB30" s="11">
         <f t="shared" si="12"/>
-        <v>7.5227721630000133</v>
+        <v>-361.44365337900012</v>
+      </c>
+      <c r="AC30" s="11">
+        <f t="shared" si="13"/>
+        <v>-365.87298723000004</v>
+      </c>
+      <c r="AD30" s="11">
+        <f t="shared" si="14"/>
+        <v>71.212471680000021</v>
+      </c>
+      <c r="AE30" s="11">
+        <f t="shared" si="15"/>
+        <v>-242.13700000000003</v>
+      </c>
+      <c r="AF30" s="11">
+        <f t="shared" si="16"/>
+        <v>4.2693338499999527</v>
       </c>
     </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>17</v>
       </c>
       <c r="C31">
-        <f t="shared" ref="C31:H31" si="22">C18-C$4</f>
-        <v>5629.5286048000007</v>
+        <f t="shared" ref="C31:H31" si="29">C18-C$4</f>
+        <v>8060.2681394800002</v>
       </c>
       <c r="D31">
-        <f t="shared" si="22"/>
-        <v>7125.2864589100009</v>
+        <f t="shared" si="29"/>
+        <v>8838.385561000001</v>
       </c>
       <c r="E31">
-        <f t="shared" si="22"/>
-        <v>7133.3886556399993</v>
+        <f t="shared" si="29"/>
+        <v>8917.3004387000001</v>
       </c>
       <c r="F31">
-        <f t="shared" si="22"/>
-        <v>-162.43600714899998</v>
+        <f t="shared" si="29"/>
+        <v>-650.64747076000003</v>
       </c>
       <c r="G31">
-        <f t="shared" si="22"/>
-        <v>1666.2960579999999</v>
+        <f t="shared" si="29"/>
+        <v>1507.63977</v>
       </c>
       <c r="H31">
-        <f t="shared" si="22"/>
-        <v>-8.1021967469999936</v>
+        <f t="shared" si="29"/>
+        <v>-79.074877723999975</v>
       </c>
       <c r="J31" t="s">
         <v>17</v>
       </c>
       <c r="K31">
+        <f t="shared" si="19"/>
+        <v>8227.6218830599992</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="20"/>
+        <v>9061.3500573000001</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="21"/>
+        <v>9140.2430847000014</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="22"/>
+        <v>-595.05856831200003</v>
+      </c>
+      <c r="O31">
         <f t="shared" si="1"/>
-        <v>5796.8823483799997</v>
-      </c>
-      <c r="L31">
+        <v>1507.63977</v>
+      </c>
+      <c r="P31">
         <f t="shared" si="2"/>
-        <v>7348.25095521</v>
-      </c>
-      <c r="M31">
-        <f t="shared" si="3"/>
-        <v>7356.3313016400007</v>
-      </c>
-      <c r="N31">
-        <f t="shared" si="4"/>
-        <v>-106.84710470099999</v>
-      </c>
-      <c r="O31">
-        <f t="shared" si="5"/>
-        <v>1666.2960579999999</v>
-      </c>
-      <c r="P31">
-        <f t="shared" si="6"/>
-        <v>-8.0803464819999817</v>
+        <v>-79.053027458999964</v>
       </c>
       <c r="R31" t="s">
         <v>17</v>
       </c>
       <c r="S31">
+        <f t="shared" si="3"/>
+        <v>2788.9086487200002</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="4"/>
+        <v>2080.7901293899995</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="5"/>
+        <v>2144.9723957599999</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="6"/>
+        <v>-527.55561296300004</v>
+      </c>
+      <c r="W31">
         <f t="shared" si="7"/>
-        <v>358.1691140400003</v>
-      </c>
-      <c r="T31">
+        <v>-116.42064000000002</v>
+      </c>
+      <c r="X31">
         <f t="shared" si="8"/>
-        <v>367.69102729999986</v>
-      </c>
-      <c r="U31">
-        <f t="shared" si="9"/>
-        <v>361.06061270000009</v>
-      </c>
-      <c r="V31">
-        <f t="shared" si="10"/>
-        <v>-39.344149351999988</v>
-      </c>
-      <c r="W31">
+        <v>-64.342266375000008</v>
+      </c>
+      <c r="Z31" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA31" s="11">
         <f t="shared" si="11"/>
-        <v>42.235647999999998</v>
-      </c>
-      <c r="X31">
+        <v>477.04346998999995</v>
+      </c>
+      <c r="AB31" s="11">
         <f t="shared" si="12"/>
-        <v>6.6304146019999735</v>
+        <v>2368.9909077299999</v>
+      </c>
+      <c r="AC31" s="11">
+        <f t="shared" si="13"/>
+        <v>2401.4893989299999</v>
+      </c>
+      <c r="AD31" s="11">
+        <f t="shared" si="14"/>
+        <v>416.76615894000008</v>
+      </c>
+      <c r="AE31" s="11">
+        <f t="shared" si="15"/>
+        <v>1507.63977</v>
+      </c>
+      <c r="AF31" s="11">
+        <f t="shared" si="16"/>
+        <v>-32.658491196</v>
+      </c>
+    </row>
+    <row r="36" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J36" s="10">
+        <v>844.020982</v>
+      </c>
+    </row>
+    <row r="37" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J41" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K21:P31">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S21:X31">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21:H31">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="7">
@@ -2870,7 +3502,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S21:X31">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA21:AF31">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2881,23 +3518,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:H31">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S21:X31">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+  <conditionalFormatting sqref="AA21:AF31">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>